<commit_message>
worked on conceptnet request
</commit_message>
<xml_diff>
--- a/Data/APNLP_QuestionsToUser.xlsx
+++ b/Data/APNLP_QuestionsToUser.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elisa\PycharmProjects\Pokerator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{701B711F-A44B-4648-BC85-73E97F754B6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE8F1414-FC17-459F-9DF1-9ED94B92221F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C52BD486-7D7C-40C5-AEA1-F1B1108B9C60}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
   <si>
     <t>Questions</t>
   </si>
@@ -63,6 +63,12 @@
   </si>
   <si>
     <t xml:space="preserve">What is your birth month? </t>
+  </si>
+  <si>
+    <t>What is your favorite music genre?</t>
+  </si>
+  <si>
+    <t>What is your favorite part of the day?</t>
   </si>
 </sst>
 </file>
@@ -414,15 +420,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7401C94A-C089-4CBC-A7AD-232C4A4D5C02}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.90625" customWidth="1"/>
+    <col min="1" max="1" width="52.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -489,6 +495,22 @@
         <v>8</v>
       </c>
     </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
merge everything part 1
</commit_message>
<xml_diff>
--- a/Data/APNLP_QuestionsToUser.xlsx
+++ b/Data/APNLP_QuestionsToUser.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elisa\PycharmProjects\Pokerator\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PyCharm\Pokerator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE8F1414-FC17-459F-9DF1-9ED94B92221F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0CCD02D-D142-4FE4-AB90-B786C408772F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C52BD486-7D7C-40C5-AEA1-F1B1108B9C60}"/>
   </bookViews>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -38,24 +36,6 @@
     <t>Questions</t>
   </si>
   <si>
-    <t>What is your favorite animal?</t>
-  </si>
-  <si>
-    <t>What is your favorite plant?</t>
-  </si>
-  <si>
-    <t>What is your hobby?</t>
-  </si>
-  <si>
-    <t>What is your favorite food?</t>
-  </si>
-  <si>
-    <t>What is your name?</t>
-  </si>
-  <si>
-    <t>What is your favorite colour?</t>
-  </si>
-  <si>
     <t>DataType</t>
   </si>
   <si>
@@ -65,10 +45,28 @@
     <t xml:space="preserve">What is your birth month? </t>
   </si>
   <si>
-    <t>What is your favorite music genre?</t>
-  </si>
-  <si>
-    <t>What is your favorite part of the day?</t>
+    <t xml:space="preserve">What is your name? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is your favorite animal? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is your favorite plant? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is your hobby? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is your favorite food? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is your favorite colour? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is your favorite music genre? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is your favorite part of the day? </t>
   </si>
 </sst>
 </file>
@@ -108,7 +106,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -124,7 +122,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -423,10 +421,10 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="52.26953125" customWidth="1"/>
   </cols>
@@ -436,63 +434,63 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
@@ -500,7 +498,7 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
@@ -508,7 +506,7 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
spaces in answers with error message removed question about favourite part of the day
</commit_message>
<xml_diff>
--- a/Data/APNLP_QuestionsToUser.xlsx
+++ b/Data/APNLP_QuestionsToUser.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PyCharm\Pokerator\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elisa\PycharmProjects\Pokerator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0CCD02D-D142-4FE4-AB90-B786C408772F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FEAA942-A9F6-4427-BDA3-1A333A6D44A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C52BD486-7D7C-40C5-AEA1-F1B1108B9C60}"/>
+    <workbookView xWindow="760" yWindow="760" windowWidth="14400" windowHeight="7360" xr2:uid="{C52BD486-7D7C-40C5-AEA1-F1B1108B9C60}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
   <si>
     <t>Questions</t>
   </si>
@@ -64,9 +64,6 @@
   </si>
   <si>
     <t xml:space="preserve">What is your favorite music genre? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">What is your favorite part of the day? </t>
   </si>
 </sst>
 </file>
@@ -106,7 +103,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -122,7 +119,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -418,13 +415,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7401C94A-C089-4CBC-A7AD-232C4A4D5C02}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="52.26953125" customWidth="1"/>
   </cols>
@@ -501,15 +498,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" t="s">
-        <v>2</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>